<commit_message>
correct speed of the ship, small changes in speed parameteres
</commit_message>
<xml_diff>
--- a/Test_Project/Test/notes/ships characteristics.xlsx
+++ b/Test_Project/Test/notes/ships characteristics.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -672,12 +672,12 @@
         <v>100</v>
       </c>
       <c r="E11">
-        <f>E2/5</f>
-        <v>2.7</v>
+        <f>1.5*E2/5</f>
+        <v>4.05</v>
       </c>
       <c r="F11">
-        <f>F2/5</f>
-        <v>1.5699999999999998</v>
+        <f>1.5*F2/5</f>
+        <v>2.3549999999999995</v>
       </c>
       <c r="G11">
         <f>G2</f>
@@ -708,12 +708,12 @@
         <v>230</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:F16" si="1">E3/5</f>
-        <v>1.9</v>
+        <f t="shared" ref="E12:F15" si="1">1.5*E3/5</f>
+        <v>2.85</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>1.05</v>
       </c>
       <c r="G12">
         <f t="shared" ref="G12:I16" si="2">G3</f>
@@ -745,11 +745,11 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>2.9</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>1.05</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
@@ -781,11 +781,11 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0.52</v>
+        <v>0.78</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
@@ -817,11 +817,11 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>3.1</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0.78</v>
+        <v>1.17</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
@@ -852,12 +852,12 @@
         <v>760</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f>1.5*E7/5</f>
+        <v>3.75</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.27999999999999997</v>
+        <f t="shared" ref="F16" si="3">1.5*F7/5</f>
+        <v>0.41999999999999993</v>
       </c>
       <c r="G16">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
fixed lot of bugs, changes in wind and model parameters
</commit_message>
<xml_diff>
--- a/Test_Project/Test/notes/ships characteristics.xlsx
+++ b/Test_Project/Test/notes/ships characteristics.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10140" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t>Model</t>
   </si>
@@ -67,13 +67,25 @@
   </si>
   <si>
     <t>With scale</t>
+  </si>
+  <si>
+    <t>Cutter</t>
+  </si>
+  <si>
+    <t>My version</t>
+  </si>
+  <si>
+    <t>Paddle speed</t>
+  </si>
+  <si>
+    <t>Jolly boat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +124,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -190,6 +207,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -224,6 +242,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -399,24 +418,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -477,7 +497,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -506,7 +526,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -535,7 +555,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -564,7 +584,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -593,7 +613,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -622,12 +642,12 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -659,7 +679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -695,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -731,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -767,7 +787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -803,7 +823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -839,7 +859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -873,6 +893,326 @@
       </c>
       <c r="J16">
         <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>500</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>15</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>18000</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="F21">
+        <v>2.355</v>
+      </c>
+      <c r="G21">
+        <v>0.9</v>
+      </c>
+      <c r="H21">
+        <v>66</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="J21">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>25000</v>
+      </c>
+      <c r="D22">
+        <v>80</v>
+      </c>
+      <c r="E22">
+        <v>3.7</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>16</v>
+      </c>
+      <c r="J22">
+        <v>20</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>38500</v>
+      </c>
+      <c r="D23">
+        <v>115</v>
+      </c>
+      <c r="E23">
+        <v>2.85</v>
+      </c>
+      <c r="F23">
+        <v>1.05</v>
+      </c>
+      <c r="G23">
+        <v>0.3</v>
+      </c>
+      <c r="H23">
+        <v>175</v>
+      </c>
+      <c r="I23">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <v>30</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>41500</v>
+      </c>
+      <c r="D24">
+        <v>135</v>
+      </c>
+      <c r="E24">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F24">
+        <v>1.05</v>
+      </c>
+      <c r="G24">
+        <v>0.4</v>
+      </c>
+      <c r="H24">
+        <v>177</v>
+      </c>
+      <c r="I24">
+        <v>16</v>
+      </c>
+      <c r="J24">
+        <v>24</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>100000</v>
+      </c>
+      <c r="D25">
+        <v>280</v>
+      </c>
+      <c r="E25">
+        <v>2.25</v>
+      </c>
+      <c r="F25">
+        <v>0.78</v>
+      </c>
+      <c r="G25">
+        <v>0.2</v>
+      </c>
+      <c r="H25">
+        <v>448</v>
+      </c>
+      <c r="I25">
+        <v>32</v>
+      </c>
+      <c r="J25">
+        <v>36</v>
+      </c>
+      <c r="K25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>150000</v>
+      </c>
+      <c r="D26">
+        <v>250</v>
+      </c>
+      <c r="E26">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F26">
+        <v>1.17</v>
+      </c>
+      <c r="G26">
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <v>323</v>
+      </c>
+      <c r="I26">
+        <v>32</v>
+      </c>
+      <c r="J26">
+        <v>46</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>250000</v>
+      </c>
+      <c r="D27">
+        <v>380</v>
+      </c>
+      <c r="E27">
+        <v>3.75</v>
+      </c>
+      <c r="F27">
+        <v>0.42</v>
+      </c>
+      <c r="G27">
+        <v>0.3</v>
+      </c>
+      <c r="H27">
+        <v>571</v>
+      </c>
+      <c r="I27">
+        <v>32</v>
+      </c>
+      <c r="J27">
+        <v>66</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -882,12 +1222,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -895,12 +1235,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Battle class + alpha version of fight function
</commit_message>
<xml_diff>
--- a/Test_Project/Test/notes/ships characteristics.xlsx
+++ b/Test_Project/Test/notes/ships characteristics.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10140" windowHeight="8055"/>
@@ -11,12 +11,12 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -79,13 +79,16 @@
   </si>
   <si>
     <t>Jolly boat</t>
+  </si>
+  <si>
+    <t>Maneuverability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,7 +210,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -242,7 +244,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -418,25 +419,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -497,7 +500,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -526,7 +529,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -555,7 +558,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -584,7 +587,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -613,7 +616,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -642,12 +645,12 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -679,7 +682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -715,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -751,7 +754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -787,7 +790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -823,7 +826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -859,7 +862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -895,12 +898,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -934,8 +937,11 @@
       <c r="K19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -964,13 +970,16 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1004,8 +1013,11 @@
       <c r="K21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1039,8 +1051,11 @@
       <c r="K22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1074,8 +1089,11 @@
       <c r="K23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1109,8 +1127,11 @@
       <c r="K24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1144,8 +1165,11 @@
       <c r="K25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1179,8 +1203,11 @@
       <c r="K26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1213,6 +1240,9 @@
       </c>
       <c r="K27">
         <v>5</v>
+      </c>
+      <c r="L27">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -1222,12 +1252,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1235,12 +1265,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>